<commit_message>
small changes for report
</commit_message>
<xml_diff>
--- a/convergence_rate.xlsx
+++ b/convergence_rate.xlsx
@@ -132,8 +132,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2400"/>
-              <a:t>Convergence rate</a:t>
+              <a:t>Training</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" baseline="0"/>
+              <a:t> curve</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2400"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2030,11 +2035,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2116947016"/>
-        <c:axId val="-2116945608"/>
+        <c:axId val="-2092116568"/>
+        <c:axId val="-2092113496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2116947016"/>
+        <c:axId val="-2092116568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2054,7 +2059,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2116945608"/>
+        <c:crossAx val="-2092113496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2063,7 +2068,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2116945608"/>
+        <c:axId val="-2092113496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.05"/>
@@ -2091,7 +2096,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2116947016"/>
+        <c:crossAx val="-2092116568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2483,7 +2488,7 @@
   <dimension ref="A1:C151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>